<commit_message>
User opera map tables in new booking report
</commit_message>
<xml_diff>
--- a/Saudi/Booking.xlsx
+++ b/Saudi/Booking.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Booking No</t>
   </si>
@@ -66,10 +66,7 @@
     <t>Purpose of Stay</t>
   </si>
   <si>
-    <t>Room</t>
-  </si>
-  <si>
-    <t>Tax</t>
+    <t>Room Tax</t>
   </si>
   <si>
     <t>DXKCV</t>
@@ -571,7 +568,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -579,12 +576,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
@@ -916,18 +907,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" style="1" customWidth="1"/>
@@ -935,11 +924,11 @@
     <col min="9" max="9" width="9.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="6.42578125" style="1" customWidth="1"/>
     <col min="11" max="11" width="6" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" style="1" customWidth="1"/>
     <col min="13" max="13" width="13.28515625" style="1" customWidth="1"/>
     <col min="14" max="14" width="11.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="6.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" style="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -989,69 +978,49 @@
       <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="4" t="s">
+      <c r="A2" s="3">
+        <v>77401</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="4">
+        <v>44279</v>
+      </c>
+      <c r="D2" s="4">
+        <v>44282</v>
+      </c>
+      <c r="E2" s="3">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3">
+        <v>401</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>77401</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="6">
-        <v>44279</v>
-      </c>
-      <c r="D3" s="6">
-        <v>44282</v>
-      </c>
-      <c r="E3" s="3">
-        <v>3</v>
-      </c>
-      <c r="F3" s="3">
-        <v>401</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="H2" s="5">
+        <v>2500</v>
+      </c>
+      <c r="I2" s="5">
+        <v>7500</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="3">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="7">
-        <v>2500</v>
-      </c>
-      <c r="I3" s="7">
-        <v>7500</v>
-      </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="3">
+      <c r="N2" s="3">
         <v>1</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" s="3">
-        <v>1</v>
-      </c>
-      <c r="O3" s="2"/>
-      <c r="P3" s="4">
+      <c r="O2" s="2"/>
+      <c r="P2" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add reservation status in create/update booking
</commit_message>
<xml_diff>
--- a/Saudi/Booking.xlsx
+++ b/Saudi/Booking.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Booking No</t>
   </si>
@@ -69,10 +69,16 @@
     <t>Room Tax</t>
   </si>
   <si>
+    <t>Resv Status</t>
+  </si>
+  <si>
     <t>DXKCV</t>
   </si>
   <si>
     <t>CA</t>
+  </si>
+  <si>
+    <t>RESERVED</t>
   </si>
 </sst>
 </file>
@@ -215,7 +221,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="6"/>
+      <sz val="5"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -907,32 +913,33 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12" style="1" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -981,8 +988,11 @@
       <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>77401</v>
       </c>
@@ -1000,7 +1010,7 @@
         <v>401</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" s="5">
         <v>2500</v>
@@ -1014,7 +1024,7 @@
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N2" s="3">
         <v>1</v>
@@ -1022,6 +1032,9 @@
       <c r="O2" s="2"/>
       <c r="P2" s="3">
         <v>0</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get booking daily and total rate
</commit_message>
<xml_diff>
--- a/Saudi/Booking.xlsx
+++ b/Saudi/Booking.xlsx
@@ -19,12 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Booking No</t>
   </si>
   <si>
-    <t>Nationality Code</t>
+    <t>Nationality</t>
   </si>
   <si>
     <t>Arrival Date</t>
@@ -42,7 +42,10 @@
     <t>Room Type</t>
   </si>
   <si>
-    <t>Full Rate Amount</t>
+    <t>Daily Rate</t>
+  </si>
+  <si>
+    <t>Total Rate</t>
   </si>
   <si>
     <t>Total Room</t>
@@ -221,7 +224,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="5"/>
+      <sz val="6"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -574,7 +577,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -582,6 +585,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="15" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
@@ -913,37 +922,38 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12" style="1" customWidth="1"/>
-    <col min="16" max="16" width="7.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="8" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6" style="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="8" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.42578125" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -991,16 +1001,19 @@
       <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>77401</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="4">
+      <c r="B2" s="4"/>
+      <c r="C2" s="6">
         <v>44279</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="6">
         <v>44282</v>
       </c>
       <c r="E2" s="3">
@@ -1010,31 +1023,34 @@
         <v>401</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="5">
+        <v>18</v>
+      </c>
+      <c r="H2" s="7">
         <v>2500</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="7">
         <v>7500</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="3">
+      <c r="J2" s="3">
+        <v>7500</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="3">
         <v>1</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="3">
+      <c r="M2" s="2"/>
+      <c r="N2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="3">
         <v>1</v>
       </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="3">
+      <c r="P2" s="2"/>
+      <c r="Q2" s="3">
         <v>0</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>19</v>
+      <c r="R2" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
get check in and checkout time for opera booking
</commit_message>
<xml_diff>
--- a/Saudi/Booking.xlsx
+++ b/Saudi/Booking.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="34">
   <si>
     <t>Booking No</t>
   </si>
@@ -33,7 +33,13 @@
     <t>Departure Date</t>
   </si>
   <si>
-    <t>Number of Nights</t>
+    <t>Arrival Time</t>
+  </si>
+  <si>
+    <t>Departure Time</t>
+  </si>
+  <si>
+    <t>Nights</t>
   </si>
   <si>
     <t>Room No.</t>
@@ -48,9 +54,6 @@
     <t>Total Rate</t>
   </si>
   <si>
-    <t>Total Room</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -60,7 +63,10 @@
     <t>Date of Birth</t>
   </si>
   <si>
-    <t>Payment Method</t>
+    <t>Pay Method</t>
+  </si>
+  <si>
+    <t>Pay Amount</t>
   </si>
   <si>
     <t>No. of Rooms</t>
@@ -72,16 +78,49 @@
     <t>Room Tax</t>
   </si>
   <si>
-    <t>Resv Status</t>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>*11:01</t>
   </si>
   <si>
     <t>DXKCV</t>
   </si>
   <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>XX/XX/XX</t>
+  </si>
+  <si>
     <t>CA</t>
   </si>
   <si>
+    <t>CHECKED IN</t>
+  </si>
+  <si>
     <t>RESERVED</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>*10:56</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>*16:45</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>Reserve Status</t>
   </si>
 </sst>
 </file>
@@ -224,7 +263,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="6"/>
+      <sz val="5"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -577,7 +616,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -593,6 +632,9 @@
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="15" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="4" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -922,34 +964,37 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6" style="1" customWidth="1"/>
+    <col min="1" max="2" width="8.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" style="1" customWidth="1"/>
+    <col min="10" max="11" width="7.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="5.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="8" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.42578125" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="13" width="5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="11" style="1" customWidth="1"/>
+    <col min="19" max="19" width="7.140625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="6.5703125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1004,55 +1049,1016 @@
       <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>77401</v>
+        <v>77904</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="6">
+        <v>43548</v>
+      </c>
+      <c r="D2" s="6">
+        <v>43551</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1106</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="3">
+        <v>459</v>
+      </c>
+      <c r="K2" s="8">
+        <v>1377</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="3">
+        <v>1</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>1</v>
+      </c>
+      <c r="R2" s="2"/>
+      <c r="S2" s="3">
+        <v>0</v>
+      </c>
+      <c r="T2" s="2"/>
+      <c r="U2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>77401</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="6">
         <v>44279</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D3" s="6">
         <v>44282</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E3" s="2"/>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
         <v>3</v>
       </c>
-      <c r="F2" s="3">
+      <c r="H3" s="3">
         <v>401</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="7">
+      <c r="I3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="8">
         <v>2500</v>
       </c>
-      <c r="I2" s="7">
+      <c r="K3" s="8">
         <v>7500</v>
       </c>
-      <c r="J2" s="3">
-        <v>7500</v>
-      </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="3">
-        <v>1</v>
-      </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="3">
-        <v>1</v>
-      </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="3">
+      <c r="L3" s="2"/>
+      <c r="M3" s="3">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="3">
         <v>0</v>
       </c>
-      <c r="R2" s="3" t="s">
-        <v>20</v>
+      <c r="Q3" s="3">
+        <v>1</v>
+      </c>
+      <c r="R3" s="2"/>
+      <c r="S3" s="3">
+        <v>0</v>
+      </c>
+      <c r="T3" s="2"/>
+      <c r="U3" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
+    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>77903</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="6">
+        <v>43548</v>
+      </c>
+      <c r="D4" s="6">
+        <v>43557</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="3">
+        <v>9</v>
+      </c>
+      <c r="H4" s="3">
+        <v>614</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="8">
+        <v>2500</v>
+      </c>
+      <c r="K4" s="8">
+        <v>22500</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="3">
+        <v>4</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>1</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" s="3">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2"/>
+      <c r="U4" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>77654</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="6">
+        <v>43548</v>
+      </c>
+      <c r="D5" s="6">
+        <v>43553</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="3">
+        <v>5</v>
+      </c>
+      <c r="H5" s="3">
+        <v>606</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="8">
+        <v>2500</v>
+      </c>
+      <c r="K5" s="8">
+        <v>12500</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="3">
+        <v>1</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" s="3">
+        <v>245</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>1</v>
+      </c>
+      <c r="R5" s="2"/>
+      <c r="S5" s="3">
+        <v>0</v>
+      </c>
+      <c r="T5" s="2"/>
+      <c r="U5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>77654</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="6">
+        <v>43548</v>
+      </c>
+      <c r="D6" s="6">
+        <v>43553</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="3">
+        <v>5</v>
+      </c>
+      <c r="H6" s="3">
+        <v>606</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="8">
+        <v>2500</v>
+      </c>
+      <c r="K6" s="8">
+        <v>12500</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="3">
+        <v>1</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P6" s="3">
+        <v>245</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>1</v>
+      </c>
+      <c r="R6" s="2"/>
+      <c r="S6" s="3">
+        <v>0</v>
+      </c>
+      <c r="T6" s="2"/>
+      <c r="U6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>77654</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="6">
+        <v>43548</v>
+      </c>
+      <c r="D7" s="6">
+        <v>43553</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="3">
+        <v>5</v>
+      </c>
+      <c r="H7" s="3">
+        <v>606</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="8">
+        <v>2500</v>
+      </c>
+      <c r="K7" s="8">
+        <v>12500</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="3">
+        <v>1</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P7" s="3">
+        <v>245</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>1</v>
+      </c>
+      <c r="R7" s="2"/>
+      <c r="S7" s="3">
+        <v>0</v>
+      </c>
+      <c r="T7" s="2"/>
+      <c r="U7" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>77654</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="6">
+        <v>43548</v>
+      </c>
+      <c r="D8" s="6">
+        <v>43553</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="3">
+        <v>5</v>
+      </c>
+      <c r="H8" s="3">
+        <v>606</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="8">
+        <v>2500</v>
+      </c>
+      <c r="K8" s="8">
+        <v>12500</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="3">
+        <v>1</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="3">
+        <v>245</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>1</v>
+      </c>
+      <c r="R8" s="2"/>
+      <c r="S8" s="3">
+        <v>0</v>
+      </c>
+      <c r="T8" s="2"/>
+      <c r="U8" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>77654</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="6">
+        <v>43548</v>
+      </c>
+      <c r="D9" s="6">
+        <v>43553</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="3">
+        <v>5</v>
+      </c>
+      <c r="H9" s="3">
+        <v>606</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="8">
+        <v>2500</v>
+      </c>
+      <c r="K9" s="8">
+        <v>12500</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="3">
+        <v>1</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P9" s="3">
+        <v>245</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>1</v>
+      </c>
+      <c r="R9" s="2"/>
+      <c r="S9" s="3">
+        <v>0</v>
+      </c>
+      <c r="T9" s="2"/>
+      <c r="U9" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>77654</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="6">
+        <v>43548</v>
+      </c>
+      <c r="D10" s="6">
+        <v>43553</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="3">
+        <v>5</v>
+      </c>
+      <c r="H10" s="3">
+        <v>606</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="8">
+        <v>2500</v>
+      </c>
+      <c r="K10" s="8">
+        <v>12500</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="3">
+        <v>1</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" s="3">
+        <v>245</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>1</v>
+      </c>
+      <c r="R10" s="2"/>
+      <c r="S10" s="3">
+        <v>0</v>
+      </c>
+      <c r="T10" s="2"/>
+      <c r="U10" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>77654</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="6">
+        <v>43548</v>
+      </c>
+      <c r="D11" s="6">
+        <v>43553</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="3">
+        <v>5</v>
+      </c>
+      <c r="H11" s="3">
+        <v>606</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="8">
+        <v>2500</v>
+      </c>
+      <c r="K11" s="8">
+        <v>12500</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="3">
+        <v>1</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P11" s="3">
+        <v>245</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>1</v>
+      </c>
+      <c r="R11" s="2"/>
+      <c r="S11" s="3">
+        <v>0</v>
+      </c>
+      <c r="T11" s="2"/>
+      <c r="U11" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>77654</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="6">
+        <v>43548</v>
+      </c>
+      <c r="D12" s="6">
+        <v>43553</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="3">
+        <v>5</v>
+      </c>
+      <c r="H12" s="3">
+        <v>606</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="8">
+        <v>2500</v>
+      </c>
+      <c r="K12" s="8">
+        <v>12500</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="3">
+        <v>1</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P12" s="3">
+        <v>245</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>1</v>
+      </c>
+      <c r="R12" s="2"/>
+      <c r="S12" s="3">
+        <v>0</v>
+      </c>
+      <c r="T12" s="2"/>
+      <c r="U12" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>77654</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="6">
+        <v>43548</v>
+      </c>
+      <c r="D13" s="6">
+        <v>43553</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G13" s="3">
+        <v>5</v>
+      </c>
+      <c r="H13" s="3">
+        <v>606</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="8">
+        <v>2500</v>
+      </c>
+      <c r="K13" s="8">
+        <v>12500</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="3">
+        <v>1</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P13" s="3">
+        <v>245</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>1</v>
+      </c>
+      <c r="R13" s="2"/>
+      <c r="S13" s="3">
+        <v>0</v>
+      </c>
+      <c r="T13" s="2"/>
+      <c r="U13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>77654</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="6">
+        <v>43548</v>
+      </c>
+      <c r="D14" s="6">
+        <v>43553</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="3">
+        <v>5</v>
+      </c>
+      <c r="H14" s="3">
+        <v>606</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="8">
+        <v>2500</v>
+      </c>
+      <c r="K14" s="8">
+        <v>12500</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="3">
+        <v>1</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P14" s="3">
+        <v>245</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>1</v>
+      </c>
+      <c r="R14" s="2"/>
+      <c r="S14" s="3">
+        <v>562.5</v>
+      </c>
+      <c r="T14" s="2"/>
+      <c r="U14" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>77654</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="6">
+        <v>43548</v>
+      </c>
+      <c r="D15" s="6">
+        <v>43553</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="3">
+        <v>5</v>
+      </c>
+      <c r="H15" s="3">
+        <v>606</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" s="8">
+        <v>2500</v>
+      </c>
+      <c r="K15" s="8">
+        <v>12500</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="3">
+        <v>1</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P15" s="3">
+        <v>245</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>1</v>
+      </c>
+      <c r="R15" s="2"/>
+      <c r="S15" s="3">
+        <v>0</v>
+      </c>
+      <c r="T15" s="2"/>
+      <c r="U15" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>77654</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="6">
+        <v>43548</v>
+      </c>
+      <c r="D16" s="6">
+        <v>43553</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="3">
+        <v>5</v>
+      </c>
+      <c r="H16" s="3">
+        <v>606</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" s="8">
+        <v>2500</v>
+      </c>
+      <c r="K16" s="8">
+        <v>12500</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="M16" s="3">
+        <v>1</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P16" s="3">
+        <v>245</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>1</v>
+      </c>
+      <c r="R16" s="2"/>
+      <c r="S16" s="3">
+        <v>0</v>
+      </c>
+      <c r="T16" s="2"/>
+      <c r="U16" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>77654</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="6">
+        <v>43548</v>
+      </c>
+      <c r="D17" s="6">
+        <v>43553</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="3">
+        <v>5</v>
+      </c>
+      <c r="H17" s="3">
+        <v>606</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="8">
+        <v>2500</v>
+      </c>
+      <c r="K17" s="8">
+        <v>12500</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="3">
+        <v>1</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P17" s="3">
+        <v>245</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>1</v>
+      </c>
+      <c r="R17" s="2"/>
+      <c r="S17" s="3">
+        <v>0</v>
+      </c>
+      <c r="T17" s="2"/>
+      <c r="U17" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>77654</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="6">
+        <v>43548</v>
+      </c>
+      <c r="D18" s="6">
+        <v>43553</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="3">
+        <v>5</v>
+      </c>
+      <c r="H18" s="3">
+        <v>606</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="8">
+        <v>2500</v>
+      </c>
+      <c r="K18" s="8">
+        <v>12500</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="3">
+        <v>1</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P18" s="3">
+        <v>245</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>1</v>
+      </c>
+      <c r="R18" s="2"/>
+      <c r="S18" s="3">
+        <v>0</v>
+      </c>
+      <c r="T18" s="2"/>
+      <c r="U18" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="15" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
OSII - WIP in fixing sync cost of goods
</commit_message>
<xml_diff>
--- a/Saudi/Booking.xlsx
+++ b/Saudi/Booking.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>Booking No</t>
   </si>
@@ -133,25 +133,13 @@
   </si>
   <si>
     <t>CL</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>FF</t>
-  </si>
-  <si>
-    <t>RC</t>
-  </si>
-  <si>
-    <t>L</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,15 +280,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="6"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -483,12 +464,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -653,7 +628,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -675,15 +650,6 @@
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="4" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1010,10 +976,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,55 +1009,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="3" t="s">
@@ -1157,9 +1123,7 @@
       <c r="Q2" s="3">
         <v>1</v>
       </c>
-      <c r="R2" s="11" t="s">
-        <v>38</v>
-      </c>
+      <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="3" t="s">
         <v>27</v>
@@ -1212,9 +1176,7 @@
       <c r="Q3" s="3">
         <v>1</v>
       </c>
-      <c r="R3" s="11" t="s">
-        <v>39</v>
-      </c>
+      <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="3" t="s">
         <v>29</v>
@@ -1275,9 +1237,7 @@
       <c r="Q4" s="3">
         <v>1</v>
       </c>
-      <c r="R4" s="11" t="s">
-        <v>40</v>
-      </c>
+      <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="3" t="s">
         <v>27</v>
@@ -1336,783 +1296,12 @@
       <c r="Q5" s="3">
         <v>1</v>
       </c>
-      <c r="R5" s="11" t="s">
-        <v>38</v>
-      </c>
+      <c r="R5" s="2"/>
       <c r="S5" s="2"/>
       <c r="T5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>77654</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="6">
-        <v>43548</v>
-      </c>
-      <c r="E6" s="6">
-        <v>43553</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="H6" s="3">
-        <v>5</v>
-      </c>
-      <c r="I6" s="3">
-        <v>606</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="8">
-        <v>2500</v>
-      </c>
-      <c r="L6" s="8">
-        <v>12500</v>
-      </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="3">
-        <v>1</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>1</v>
-      </c>
-      <c r="R6" s="11"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U6" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>77654</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="6">
-        <v>43548</v>
-      </c>
-      <c r="E7" s="6">
-        <v>43553</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="H7" s="3">
-        <v>5</v>
-      </c>
-      <c r="I7" s="3">
-        <v>606</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="8">
-        <v>2500</v>
-      </c>
-      <c r="L7" s="8">
-        <v>12500</v>
-      </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="3">
-        <v>1</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q7" s="3">
-        <v>1</v>
-      </c>
-      <c r="R7" s="11"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U7" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>77654</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="6">
-        <v>43548</v>
-      </c>
-      <c r="E8" s="6">
-        <v>43553</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="H8" s="3">
-        <v>5</v>
-      </c>
-      <c r="I8" s="3">
-        <v>606</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="8">
-        <v>2500</v>
-      </c>
-      <c r="L8" s="8">
-        <v>12500</v>
-      </c>
-      <c r="M8" s="2"/>
-      <c r="N8" s="3">
-        <v>1</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q8" s="3">
-        <v>1</v>
-      </c>
-      <c r="R8" s="11"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U8" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>77654</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="6">
-        <v>43548</v>
-      </c>
-      <c r="E9" s="6">
-        <v>43553</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="H9" s="3">
-        <v>5</v>
-      </c>
-      <c r="I9" s="3">
-        <v>606</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="8">
-        <v>2500</v>
-      </c>
-      <c r="L9" s="8">
-        <v>12500</v>
-      </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="3">
-        <v>1</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q9" s="3">
-        <v>1</v>
-      </c>
-      <c r="R9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="S9" s="2"/>
-      <c r="T9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U9" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>77654</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="6">
-        <v>43548</v>
-      </c>
-      <c r="E10" s="6">
-        <v>43553</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="H10" s="3">
-        <v>5</v>
-      </c>
-      <c r="I10" s="3">
-        <v>606</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="8">
-        <v>2500</v>
-      </c>
-      <c r="L10" s="8">
-        <v>12500</v>
-      </c>
-      <c r="M10" s="2"/>
-      <c r="N10" s="3">
-        <v>1</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q10" s="3">
-        <v>1</v>
-      </c>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U10" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>77654</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="6">
-        <v>43548</v>
-      </c>
-      <c r="E11" s="6">
-        <v>43553</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="H11" s="3">
-        <v>5</v>
-      </c>
-      <c r="I11" s="3">
-        <v>606</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" s="8">
-        <v>2500</v>
-      </c>
-      <c r="L11" s="8">
-        <v>12500</v>
-      </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="3">
-        <v>1</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q11" s="3">
-        <v>1</v>
-      </c>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U11" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>77654</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="6">
-        <v>43548</v>
-      </c>
-      <c r="E12" s="6">
-        <v>43553</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="H12" s="3">
-        <v>5</v>
-      </c>
-      <c r="I12" s="3">
-        <v>606</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="8">
-        <v>2500</v>
-      </c>
-      <c r="L12" s="8">
-        <v>12500</v>
-      </c>
-      <c r="M12" s="2"/>
-      <c r="N12" s="3">
-        <v>1</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q12" s="3">
-        <v>1</v>
-      </c>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U12" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>77654</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="6">
-        <v>43548</v>
-      </c>
-      <c r="E13" s="6">
-        <v>43553</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="H13" s="3">
-        <v>5</v>
-      </c>
-      <c r="I13" s="3">
-        <v>606</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="8">
-        <v>2500</v>
-      </c>
-      <c r="L13" s="8">
-        <v>12500</v>
-      </c>
-      <c r="M13" s="2"/>
-      <c r="N13" s="3">
-        <v>1</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q13" s="3">
-        <v>1</v>
-      </c>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U13" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>77654</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="6">
-        <v>43548</v>
-      </c>
-      <c r="E14" s="6">
-        <v>43553</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="H14" s="3">
-        <v>5</v>
-      </c>
-      <c r="I14" s="3">
-        <v>606</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K14" s="8">
-        <v>2500</v>
-      </c>
-      <c r="L14" s="8">
-        <v>12500</v>
-      </c>
-      <c r="M14" s="2"/>
-      <c r="N14" s="3">
-        <v>1</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q14" s="3">
-        <v>1</v>
-      </c>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U14" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>77654</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="6">
-        <v>43548</v>
-      </c>
-      <c r="E15" s="6">
-        <v>43553</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="H15" s="3">
-        <v>5</v>
-      </c>
-      <c r="I15" s="3">
-        <v>606</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" s="8">
-        <v>2500</v>
-      </c>
-      <c r="L15" s="8">
-        <v>12500</v>
-      </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="3">
-        <v>1</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q15" s="3">
-        <v>1</v>
-      </c>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U15" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>77654</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="6">
-        <v>43548</v>
-      </c>
-      <c r="E16" s="6">
-        <v>43553</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="H16" s="3">
-        <v>5</v>
-      </c>
-      <c r="I16" s="3">
-        <v>606</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K16" s="8">
-        <v>2500</v>
-      </c>
-      <c r="L16" s="8">
-        <v>12500</v>
-      </c>
-      <c r="M16" s="2"/>
-      <c r="N16" s="3">
-        <v>1</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q16" s="3">
-        <v>1</v>
-      </c>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U16" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>77654</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="6">
-        <v>43548</v>
-      </c>
-      <c r="E17" s="6">
-        <v>43553</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="H17" s="3">
-        <v>5</v>
-      </c>
-      <c r="I17" s="3">
-        <v>606</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="8">
-        <v>2500</v>
-      </c>
-      <c r="L17" s="8">
-        <v>12500</v>
-      </c>
-      <c r="M17" s="2"/>
-      <c r="N17" s="3">
-        <v>1</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q17" s="3">
-        <v>1</v>
-      </c>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U17" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>77654</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="6">
-        <v>43548</v>
-      </c>
-      <c r="E18" s="6">
-        <v>43553</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="H18" s="3">
-        <v>5</v>
-      </c>
-      <c r="I18" s="3">
-        <v>606</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K18" s="8">
-        <v>2500</v>
-      </c>
-      <c r="L18" s="8">
-        <v>12500</v>
-      </c>
-      <c r="M18" s="2"/>
-      <c r="N18" s="3">
-        <v>1</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q18" s="3">
-        <v>1</v>
-      </c>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U18" s="3" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
OPERA Report - Read BD of user in new booking
</commit_message>
<xml_diff>
--- a/Saudi/Booking.xlsx
+++ b/Saudi/Booking.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>Booking No</t>
   </si>
@@ -84,46 +84,52 @@
     <t>Rate Code</t>
   </si>
   <si>
+    <t>GC</t>
+  </si>
+  <si>
+    <t>*15:07</t>
+  </si>
+  <si>
+    <t>DXKCV</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>CHECKED IN</t>
+  </si>
+  <si>
+    <t>BARRO</t>
+  </si>
+  <si>
     <t>RS</t>
   </si>
   <si>
     <t>*11:01</t>
   </si>
   <si>
-    <t>DXKCV</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>XX/XX/XX</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>CHECKED IN</t>
-  </si>
-  <si>
-    <t>BARRO</t>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>VS</t>
+  </si>
+  <si>
+    <t>*10:56</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>RACK</t>
   </si>
   <si>
     <t>RESERVED</t>
-  </si>
-  <si>
-    <t>RACK</t>
-  </si>
-  <si>
-    <t>AD</t>
-  </si>
-  <si>
-    <t>VS</t>
-  </si>
-  <si>
-    <t>*10:56</t>
-  </si>
-  <si>
-    <t>F</t>
   </si>
   <si>
     <t>AE</t>
@@ -976,17 +982,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="3.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="1" customWidth="1"/>
@@ -1004,11 +1010,11 @@
     <col min="18" max="18" width="4.140625" style="1" customWidth="1"/>
     <col min="19" max="19" width="7" style="1" customWidth="1"/>
     <col min="20" max="20" width="9.85546875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.140625" style="1" customWidth="1"/>
     <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1073,9 +1079,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>77904</v>
+        <v>77905</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="3" t="s">
@@ -1085,45 +1091,45 @@
         <v>43548</v>
       </c>
       <c r="E2" s="6">
-        <v>43551</v>
+        <v>43571</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G2" s="7">
-        <v>0.20833333333333334</v>
+        <v>0.25</v>
       </c>
       <c r="H2" s="3">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="I2" s="3">
-        <v>1106</v>
+        <v>1209</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>23</v>
       </c>
       <c r="K2" s="3">
-        <v>459</v>
+        <v>464.1</v>
       </c>
       <c r="L2" s="8">
-        <v>1377</v>
+        <v>10674.3</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>24</v>
       </c>
       <c r="N2" s="3">
-        <v>1</v>
-      </c>
-      <c r="O2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="Q2" s="3">
         <v>1</v>
       </c>
-      <c r="R2" s="2"/>
+      <c r="R2" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="S2" s="2"/>
       <c r="T2" s="3" t="s">
         <v>27</v>
@@ -1132,46 +1138,52 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>77401</v>
+        <v>77904</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="3" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="D3" s="6">
-        <v>44279</v>
+        <v>43548</v>
       </c>
       <c r="E3" s="6">
-        <v>44282</v>
-      </c>
-      <c r="F3" s="2"/>
+        <v>43551</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="G3" s="7">
-        <v>0</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="H3" s="3">
         <v>3</v>
       </c>
       <c r="I3" s="3">
-        <v>401</v>
+        <v>1106</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="8">
-        <v>2500</v>
+      <c r="K3" s="3">
+        <v>459</v>
       </c>
       <c r="L3" s="8">
-        <v>7500</v>
-      </c>
-      <c r="M3" s="2"/>
+        <v>1377</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="N3" s="3">
         <v>1</v>
       </c>
-      <c r="O3" s="2"/>
+      <c r="O3" s="6">
+        <v>43525</v>
+      </c>
       <c r="P3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q3" s="3">
         <v>1</v>
@@ -1179,13 +1191,13 @@
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>77903</v>
       </c>
@@ -1228,11 +1240,11 @@
       <c r="N4" s="3">
         <v>4</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="6">
+        <v>36220</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="Q4" s="3">
         <v>1</v>
@@ -1243,36 +1255,32 @@
         <v>27</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>77654</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>35</v>
-      </c>
+        <v>77401</v>
+      </c>
+      <c r="B5" s="4"/>
       <c r="C5" s="3" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D5" s="6">
-        <v>43548</v>
+        <v>44279</v>
       </c>
       <c r="E5" s="6">
-        <v>43553</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>44282</v>
+      </c>
+      <c r="F5" s="2"/>
       <c r="G5" s="7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H5" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I5" s="3">
-        <v>606</v>
+        <v>401</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>23</v>
@@ -1281,17 +1289,15 @@
         <v>2500</v>
       </c>
       <c r="L5" s="8">
-        <v>12500</v>
+        <v>7500</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="3">
         <v>1</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="2"/>
+      <c r="P5" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="Q5" s="3">
         <v>1</v>
@@ -1299,10 +1305,69 @@
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
       <c r="T5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>77654</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="6">
+        <v>43548</v>
+      </c>
+      <c r="E6" s="6">
+        <v>43553</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="3">
+        <v>5</v>
+      </c>
+      <c r="I6" s="3">
+        <v>606</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="8">
+        <v>2500</v>
+      </c>
+      <c r="L6" s="8">
+        <v>12500</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="3">
+        <v>1</v>
+      </c>
+      <c r="O6" s="6">
+        <v>28836</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>1</v>
+      </c>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="U5" s="3" t="s">
-        <v>30</v>
+      <c r="U6" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OPERA Reports - WIP in fix calc room rent type
</commit_message>
<xml_diff>
--- a/Saudi/Booking.xlsx
+++ b/Saudi/Booking.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="56">
   <si>
     <t>Booking No</t>
   </si>
@@ -39,106 +39,154 @@
     <t>Arrival Time</t>
   </si>
   <si>
+    <t>Nights</t>
+  </si>
+  <si>
+    <t>Room No.</t>
+  </si>
+  <si>
+    <t>Room Type</t>
+  </si>
+  <si>
+    <t>Daily Rate</t>
+  </si>
+  <si>
+    <t>Total Rate</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Adults</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Pay Method</t>
+  </si>
+  <si>
+    <t>POS</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Discount Percent</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Rate Code</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>07.05.21</t>
+  </si>
+  <si>
+    <t>08.05.21</t>
+  </si>
+  <si>
+    <t>DLX01K</t>
+  </si>
+  <si>
+    <t>31.12.90</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>CHECKED OUT</t>
+  </si>
+  <si>
+    <t>BARBB</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>14.05.21</t>
+  </si>
+  <si>
+    <t>15.05.21</t>
+  </si>
+  <si>
+    <t>RESERVED</t>
+  </si>
+  <si>
+    <t>27.05.21</t>
+  </si>
+  <si>
+    <t>29.05.21</t>
+  </si>
+  <si>
+    <t>STEG1K</t>
+  </si>
+  <si>
+    <t>SPAN</t>
+  </si>
+  <si>
+    <t>AX</t>
+  </si>
+  <si>
+    <t>DLX02S</t>
+  </si>
+  <si>
+    <t>RAMADAND</t>
+  </si>
+  <si>
+    <t>*02:51</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>PK004BBB</t>
+  </si>
+  <si>
+    <t>26.05.21</t>
+  </si>
+  <si>
+    <t>28.05.21</t>
+  </si>
+  <si>
+    <t>UP00390R</t>
+  </si>
+  <si>
+    <t>13.05.21</t>
+  </si>
+  <si>
+    <t>CHECKED IN</t>
+  </si>
+  <si>
+    <t>PK04972B</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>18.05.21</t>
+  </si>
+  <si>
+    <t>20.05.21</t>
+  </si>
+  <si>
+    <t>UD02938R</t>
+  </si>
+  <si>
     <t>Departure Time</t>
   </si>
   <si>
-    <t>Nights</t>
-  </si>
-  <si>
-    <t>Room No.</t>
-  </si>
-  <si>
-    <t>Room Type</t>
-  </si>
-  <si>
-    <t>Daily Rate</t>
-  </si>
-  <si>
-    <t>Total Rate</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Adults</t>
-  </si>
-  <si>
-    <t>Date of Birth</t>
-  </si>
-  <si>
-    <t>Pay Method</t>
-  </si>
-  <si>
     <t>No. of Rooms</t>
-  </si>
-  <si>
-    <t>POS</t>
-  </si>
-  <si>
-    <t>Discount</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Rate Code</t>
-  </si>
-  <si>
-    <t>GC</t>
-  </si>
-  <si>
-    <t>*15:07</t>
-  </si>
-  <si>
-    <t>DXKCV</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>CHECKED IN</t>
-  </si>
-  <si>
-    <t>BARRO</t>
-  </si>
-  <si>
-    <t>RS</t>
-  </si>
-  <si>
-    <t>*11:01</t>
-  </si>
-  <si>
-    <t>AD</t>
-  </si>
-  <si>
-    <t>VS</t>
-  </si>
-  <si>
-    <t>*10:56</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>RACK</t>
-  </si>
-  <si>
-    <t>RESERVED</t>
-  </si>
-  <si>
-    <t>AE</t>
-  </si>
-  <si>
-    <t>*16:45</t>
-  </si>
-  <si>
-    <t>CL</t>
   </si>
 </sst>
 </file>
@@ -281,7 +329,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="6"/>
+      <sz val="5"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -634,7 +682,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -648,9 +696,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="20" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
@@ -982,39 +1027,38 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="5.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="5.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="4.140625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="7" style="1" customWidth="1"/>
-    <col min="20" max="20" width="9.85546875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10.140625" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="8.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8" style="1" customWidth="1"/>
+    <col min="11" max="12" width="7.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="5.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5703125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="3.85546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="6.5703125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.28515625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1034,154 +1078,152 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>971469</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>77905</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="6">
-        <v>43548</v>
-      </c>
-      <c r="E2" s="6">
-        <v>43571</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="7">
-        <v>0.25</v>
+      <c r="F2" s="6">
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.21111111111111111</v>
       </c>
       <c r="H2" s="3">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="I2" s="3">
-        <v>1209</v>
+        <v>248</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>23</v>
       </c>
       <c r="K2" s="3">
-        <v>464.1</v>
-      </c>
-      <c r="L2" s="8">
-        <v>10674.3</v>
-      </c>
-      <c r="M2" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="L2" s="3">
+        <v>400</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="3">
+        <v>1</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="3">
-        <v>2</v>
-      </c>
-      <c r="O2" s="2"/>
       <c r="P2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="Q2" s="3">
         <v>1</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="2"/>
-      <c r="T2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="U2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>971219</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>77904</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="6">
-        <v>43548</v>
-      </c>
-      <c r="E3" s="6">
-        <v>43551</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="7">
-        <v>0.20833333333333334</v>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.54097222222222219</v>
       </c>
       <c r="H3" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I3" s="3">
-        <v>1106</v>
+        <v>110</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>23</v>
       </c>
       <c r="K3" s="3">
-        <v>459</v>
-      </c>
-      <c r="L3" s="8">
-        <v>1377</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>450</v>
+      </c>
+      <c r="L3" s="3">
+        <v>450</v>
+      </c>
+      <c r="M3" s="2"/>
       <c r="N3" s="3">
-        <v>1</v>
-      </c>
-      <c r="O3" s="6">
-        <v>43525</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="O3" s="2"/>
       <c r="P3" s="3" t="s">
         <v>25</v>
       </c>
@@ -1190,59 +1232,54 @@
       </c>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
-      <c r="T3" s="3" t="s">
+      <c r="T3" s="2"/>
+      <c r="U3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="U3" s="3" t="s">
-        <v>28</v>
-      </c>
     </row>
-    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>77903</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="6">
-        <v>43548</v>
-      </c>
-      <c r="E4" s="6">
-        <v>43557</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="7">
-        <v>0.5</v>
+        <v>969469</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.63611111111111118</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.60763888888888895</v>
       </c>
       <c r="H4" s="3">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I4" s="3">
-        <v>614</v>
+        <v>9050</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="8">
-        <v>2500</v>
-      </c>
-      <c r="L4" s="8">
-        <v>22500</v>
+        <v>29</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="N4" s="3">
-        <v>4</v>
-      </c>
-      <c r="O4" s="6">
-        <v>36220</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O4" s="2"/>
       <c r="P4" s="3" t="s">
         <v>25</v>
       </c>
@@ -1251,49 +1288,52 @@
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
-      <c r="T4" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="T4" s="2"/>
       <c r="U4" s="3" t="s">
-        <v>35</v>
+        <v>26</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>77401</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="6">
-        <v>44279</v>
-      </c>
-      <c r="E5" s="6">
-        <v>44282</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="7">
-        <v>0</v>
+        <v>967469</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.35347222222222219</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.77916666666666667</v>
       </c>
       <c r="H5" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I5" s="3">
-        <v>401</v>
+        <v>208</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="8">
-        <v>2500</v>
-      </c>
-      <c r="L5" s="8">
-        <v>7500</v>
+      <c r="K5" s="3">
+        <v>450</v>
+      </c>
+      <c r="L5" s="3">
+        <v>450</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" s="3" t="s">
@@ -1304,74 +1344,843 @@
       </c>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
-      <c r="T5" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="T5" s="2"/>
       <c r="U5" s="3" t="s">
-        <v>35</v>
+        <v>26</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>77654</v>
+        <v>967969</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="6">
-        <v>43548</v>
-      </c>
-      <c r="E6" s="6">
-        <v>43553</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="7">
-        <v>0.5</v>
+        <v>28</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.4284722222222222</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.57777777777777783</v>
       </c>
       <c r="H6" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I6" s="3">
-        <v>606</v>
+        <v>105</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="8">
-        <v>2500</v>
-      </c>
-      <c r="L6" s="8">
-        <v>12500</v>
+      <c r="K6" s="3">
+        <v>450</v>
+      </c>
+      <c r="L6" s="3">
+        <v>450</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="3">
-        <v>1</v>
-      </c>
-      <c r="O6" s="6">
-        <v>28836</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="O6" s="2"/>
       <c r="P6" s="3" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="Q6" s="3">
         <v>1</v>
       </c>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
-      <c r="T6" s="3" t="s">
+      <c r="T6" s="2"/>
+      <c r="U6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="U6" s="3" t="s">
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>968969</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <v>244</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="3">
+        <v>650</v>
+      </c>
+      <c r="L7" s="3">
+        <v>650</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="3">
+        <v>2</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>1</v>
+      </c>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>968719</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>35</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3">
+        <v>252</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="7">
+        <v>2200</v>
+      </c>
+      <c r="L8" s="7">
+        <v>4400</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="3">
+        <v>2</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>1</v>
+      </c>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>968220</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.4597222222222222</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <v>103</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="3">
+        <v>400</v>
+      </c>
+      <c r="L9" s="3">
+        <v>400</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" s="3">
+        <v>1</v>
+      </c>
+      <c r="O9" s="2"/>
+      <c r="P9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>1</v>
+      </c>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>968219</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.45902777777777781</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.44027777777777777</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>146</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="3">
+        <v>400</v>
+      </c>
+      <c r="L10" s="3">
+        <v>400</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" s="3">
+        <v>1</v>
+      </c>
+      <c r="O10" s="2"/>
+      <c r="P10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>1</v>
+      </c>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>969719</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.65208333333333335</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.4597222222222222</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3">
+        <v>145</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11" s="3">
+        <v>610</v>
+      </c>
+      <c r="L11" s="3">
+        <v>610</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="3">
+        <v>3</v>
+      </c>
+      <c r="O11" s="2"/>
+      <c r="P11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>1</v>
+      </c>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>970719</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.66249999999999998</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
+      <c r="I12" s="3">
+        <v>135</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="3">
+        <v>405</v>
+      </c>
+      <c r="L12" s="3">
+        <v>405</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" s="3">
+        <v>2</v>
+      </c>
+      <c r="O12" s="2"/>
+      <c r="P12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>1</v>
+      </c>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>970219</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="6">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3">
+        <v>2</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="3">
+        <v>550</v>
+      </c>
+      <c r="L13" s="7">
+        <v>1100</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" s="3">
+        <v>2</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>1</v>
+      </c>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>967719</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.78263888888888899</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3">
+        <v>140</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="3">
+        <v>405</v>
+      </c>
+      <c r="L14" s="3">
+        <v>405</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N14" s="3">
+        <v>2</v>
+      </c>
+      <c r="O14" s="2"/>
+      <c r="P14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>1</v>
+      </c>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>966722</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0.9375</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>5</v>
+      </c>
+      <c r="I15" s="3">
+        <v>148</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" s="3">
+        <v>400</v>
+      </c>
+      <c r="L15" s="7">
+        <v>2000</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N15" s="3">
+        <v>1</v>
+      </c>
+      <c r="O15" s="2"/>
+      <c r="P15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>1</v>
+      </c>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>966721</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0.96527777777777779</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0.46111111111111108</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3">
+        <v>222</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="3">
+        <v>400</v>
+      </c>
+      <c r="L16" s="3">
+        <v>400</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N16" s="3">
+        <v>1</v>
+      </c>
+      <c r="O16" s="2"/>
+      <c r="P16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>1</v>
+      </c>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>966720</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0.96458333333333324</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0.65625</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1</v>
+      </c>
+      <c r="I17" s="3">
+        <v>221</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="3">
+        <v>400</v>
+      </c>
+      <c r="L17" s="3">
+        <v>400</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N17" s="3">
+        <v>1</v>
+      </c>
+      <c r="O17" s="2"/>
+      <c r="P17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>1</v>
+      </c>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V17" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>966719</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0.96458333333333324</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3">
+        <v>219</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="3">
+        <v>400</v>
+      </c>
+      <c r="L18" s="3">
+        <v>400</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N18" s="3">
+        <v>1</v>
+      </c>
+      <c r="O18" s="2"/>
+      <c r="P18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>1</v>
+      </c>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>966470</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="6">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
+        <v>2</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K19" s="3">
+        <v>650</v>
+      </c>
+      <c r="L19" s="7">
+        <v>1300</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N19" s="3">
+        <v>2</v>
+      </c>
+      <c r="O19" s="2"/>
+      <c r="P19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>1</v>
+      </c>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V19" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>966469</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="6">
+        <v>0</v>
+      </c>
+      <c r="H20" s="3">
+        <v>2</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="3">
+        <v>495</v>
+      </c>
+      <c r="L20" s="3">
+        <v>990</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N20" s="3">
+        <v>2</v>
+      </c>
+      <c r="O20" s="2"/>
+      <c r="P20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>1</v>
+      </c>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V20" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
OPERA Report - check if there any update in booking
</commit_message>
<xml_diff>
--- a/Saudi/Booking.xlsx
+++ b/Saudi/Booking.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11445"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="20">
-  <si>
-    <t>Birth Date</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="25">
   <si>
     <t>Gender</t>
   </si>
@@ -45,19 +42,25 @@
     <t>Pos</t>
   </si>
   <si>
-    <t>Payment Method</t>
-  </si>
-  <si>
-    <t>Reservation Date</t>
+    <t>Pm</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>Res Date</t>
   </si>
   <si>
     <t>Amount</t>
   </si>
   <si>
-    <t>Discount</t>
-  </si>
-  <si>
-    <t>Discount Prcnt</t>
+    <t>Disc</t>
+  </si>
+  <si>
+    <t>Disc Prcnt</t>
   </si>
   <si>
     <t>Adults</t>
@@ -66,16 +69,28 @@
     <t>Children</t>
   </si>
   <si>
+    <t>Birth</t>
+  </si>
+  <si>
+    <t>VS</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>RESERVED</t>
+  </si>
+  <si>
     <t>F</t>
   </si>
   <si>
     <t>AE</t>
   </si>
   <si>
-    <t>GC</t>
-  </si>
-  <si>
-    <t>T</t>
+    <t>RS</t>
   </si>
   <si>
     <t>VI</t>
@@ -937,31 +952,35 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="13" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11" style="1" customWidth="1"/>
+    <col min="17" max="17" width="8.85546875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1007,366 +1026,690 @@
       <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="4">
+      <c r="B2" s="3"/>
+      <c r="C2" s="4">
+        <v>24926</v>
+      </c>
+      <c r="D2" s="5">
+        <v>43548</v>
+      </c>
+      <c r="E2" s="5">
+        <v>43553</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="5">
+        <v>43548</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0</v>
+      </c>
+      <c r="O2" s="4">
+        <v>1</v>
+      </c>
+      <c r="P2" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3"/>
+    </row>
+    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4">
+        <v>24926</v>
+      </c>
+      <c r="D3" s="5">
+        <v>43548</v>
+      </c>
+      <c r="E3" s="5">
+        <v>43553</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="5">
+        <v>43549</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0</v>
+      </c>
+      <c r="O3" s="4">
+        <v>1</v>
+      </c>
+      <c r="P3" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3"/>
+    </row>
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4">
+        <v>24926</v>
+      </c>
+      <c r="D4" s="5">
+        <v>43548</v>
+      </c>
+      <c r="E4" s="5">
+        <v>43553</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="5">
+        <v>43550</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>1</v>
+      </c>
+      <c r="P4" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3"/>
+    </row>
+    <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4">
+        <v>24926</v>
+      </c>
+      <c r="D5" s="5">
+        <v>43548</v>
+      </c>
+      <c r="E5" s="5">
+        <v>43553</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="5">
+        <v>43551</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0</v>
+      </c>
+      <c r="O5" s="4">
+        <v>1</v>
+      </c>
+      <c r="P5" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3"/>
+    </row>
+    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4">
+        <v>24926</v>
+      </c>
+      <c r="D6" s="5">
+        <v>43548</v>
+      </c>
+      <c r="E6" s="5">
+        <v>43553</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="5">
+        <v>43552</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0</v>
+      </c>
+      <c r="O6" s="4">
+        <v>1</v>
+      </c>
+      <c r="P6" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3"/>
+    </row>
+    <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4">
+        <v>24926</v>
+      </c>
+      <c r="D7" s="5">
+        <v>43548</v>
+      </c>
+      <c r="E7" s="5">
+        <v>43553</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="5">
+        <v>43553</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0</v>
+      </c>
+      <c r="O7" s="4">
+        <v>1</v>
+      </c>
+      <c r="P7" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3"/>
+    </row>
+    <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4">
         <v>24903</v>
       </c>
-      <c r="E2" s="5">
+      <c r="D8" s="5">
         <v>43737</v>
       </c>
-      <c r="F2" s="5">
+      <c r="E8" s="5">
         <v>43744</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="F8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="5">
+      <c r="H8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="4">
+        <v>401</v>
+      </c>
+      <c r="K8" s="5">
         <v>43737</v>
       </c>
-      <c r="K2" s="4">
+      <c r="L8" s="4">
         <v>636.98</v>
       </c>
-      <c r="L2" s="4">
-        <v>0</v>
-      </c>
-      <c r="M2" s="4">
-        <v>0</v>
-      </c>
-      <c r="N2" s="4">
+      <c r="M8" s="4">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
+      <c r="O8" s="4">
         <v>2</v>
       </c>
-      <c r="O2" s="4">
-        <v>0</v>
-      </c>
+      <c r="P8" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3"/>
     </row>
-    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="4">
+    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="4">
         <v>24903</v>
       </c>
-      <c r="E3" s="5">
+      <c r="D9" s="5">
         <v>43737</v>
       </c>
-      <c r="F3" s="5">
+      <c r="E9" s="5">
         <v>43744</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="F9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="5">
+      <c r="H9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="4">
+        <v>401</v>
+      </c>
+      <c r="K9" s="5">
         <v>43738</v>
       </c>
-      <c r="K3" s="4">
+      <c r="L9" s="4">
         <v>636.98</v>
       </c>
-      <c r="L3" s="4">
-        <v>0</v>
-      </c>
-      <c r="M3" s="4">
-        <v>0</v>
-      </c>
-      <c r="N3" s="4">
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0</v>
+      </c>
+      <c r="O9" s="4">
         <v>2</v>
       </c>
-      <c r="O3" s="4">
-        <v>0</v>
-      </c>
+      <c r="P9" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3"/>
     </row>
-    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="4">
+    <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="4">
         <v>24903</v>
       </c>
-      <c r="E4" s="5">
+      <c r="D10" s="5">
         <v>43737</v>
       </c>
-      <c r="F4" s="5">
+      <c r="E10" s="5">
         <v>43744</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="4" t="s">
+      <c r="F10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="5">
+      <c r="H10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="4">
+        <v>401</v>
+      </c>
+      <c r="K10" s="5">
         <v>43739</v>
       </c>
-      <c r="K4" s="4">
+      <c r="L10" s="4">
         <v>696.83</v>
       </c>
-      <c r="L4" s="4">
-        <v>0</v>
-      </c>
-      <c r="M4" s="4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="4">
+      <c r="M10" s="4">
+        <v>0</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+      <c r="O10" s="4">
         <v>2</v>
       </c>
-      <c r="O4" s="4">
-        <v>0</v>
-      </c>
+      <c r="P10" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="3"/>
     </row>
-    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="4">
+    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="4">
         <v>24903</v>
       </c>
-      <c r="E5" s="5">
+      <c r="D11" s="5">
         <v>43737</v>
       </c>
-      <c r="F5" s="5">
+      <c r="E11" s="5">
         <v>43744</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="4" t="s">
+      <c r="F11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="5">
+      <c r="H11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="4">
+        <v>401</v>
+      </c>
+      <c r="K11" s="5">
         <v>43740</v>
       </c>
-      <c r="K5" s="4">
+      <c r="L11" s="4">
         <v>696.83</v>
       </c>
-      <c r="L5" s="4">
-        <v>0</v>
-      </c>
-      <c r="M5" s="4">
-        <v>0</v>
-      </c>
-      <c r="N5" s="4">
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
+      <c r="O11" s="4">
         <v>2</v>
       </c>
-      <c r="O5" s="4">
-        <v>0</v>
-      </c>
+      <c r="P11" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="3"/>
     </row>
-    <row r="6" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="4">
+    <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="4">
         <v>24903</v>
       </c>
-      <c r="E6" s="5">
+      <c r="D12" s="5">
         <v>43737</v>
       </c>
-      <c r="F6" s="5">
+      <c r="E12" s="5">
         <v>43744</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="4" t="s">
+      <c r="F12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="5">
+      <c r="H12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="4">
+        <v>401</v>
+      </c>
+      <c r="K12" s="5">
         <v>43741</v>
       </c>
-      <c r="K6" s="4">
+      <c r="L12" s="4">
         <v>696.83</v>
       </c>
-      <c r="L6" s="4">
-        <v>0</v>
-      </c>
-      <c r="M6" s="4">
-        <v>0</v>
-      </c>
-      <c r="N6" s="4">
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <v>0</v>
+      </c>
+      <c r="O12" s="4">
         <v>2</v>
       </c>
-      <c r="O6" s="4">
-        <v>0</v>
-      </c>
+      <c r="P12" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="3"/>
     </row>
-    <row r="7" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="4">
+    <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="4">
         <v>24903</v>
       </c>
-      <c r="E7" s="5">
+      <c r="D13" s="5">
         <v>43737</v>
       </c>
-      <c r="F7" s="5">
+      <c r="E13" s="5">
         <v>43744</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="4" t="s">
+      <c r="F13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="5">
+      <c r="H13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="4">
+        <v>401</v>
+      </c>
+      <c r="K13" s="5">
         <v>43742</v>
       </c>
-      <c r="K7" s="4">
+      <c r="L13" s="4">
         <v>696.83</v>
       </c>
-      <c r="L7" s="4">
-        <v>0</v>
-      </c>
-      <c r="M7" s="4">
-        <v>0</v>
-      </c>
-      <c r="N7" s="4">
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4">
         <v>2</v>
       </c>
-      <c r="O7" s="4">
-        <v>0</v>
-      </c>
+      <c r="P13" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="3"/>
     </row>
-    <row r="8" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="4">
+    <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4">
         <v>24903</v>
       </c>
-      <c r="E8" s="5">
+      <c r="D14" s="5">
         <v>43737</v>
       </c>
-      <c r="F8" s="5">
+      <c r="E14" s="5">
         <v>43744</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="F14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="5">
+      <c r="H14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="4">
+        <v>401</v>
+      </c>
+      <c r="K14" s="5">
         <v>43743</v>
       </c>
-      <c r="K8" s="4">
+      <c r="L14" s="4">
         <v>696.83</v>
       </c>
-      <c r="L8" s="4">
-        <v>0</v>
-      </c>
-      <c r="M8" s="4">
-        <v>0</v>
-      </c>
-      <c r="N8" s="4">
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0</v>
+      </c>
+      <c r="O14" s="4">
         <v>2</v>
       </c>
-      <c r="O8" s="4">
-        <v>0</v>
-      </c>
+      <c r="P14" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="3"/>
     </row>
-    <row r="9" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="4">
+    <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="4">
         <v>24903</v>
       </c>
-      <c r="E9" s="5">
+      <c r="D15" s="5">
         <v>43737</v>
       </c>
-      <c r="F9" s="5">
+      <c r="E15" s="5">
         <v>43744</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="F15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="5">
+      <c r="H15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="4">
+        <v>401</v>
+      </c>
+      <c r="K15" s="5">
         <v>43744</v>
       </c>
-      <c r="K9" s="4">
+      <c r="L15" s="4">
         <v>696.83</v>
       </c>
-      <c r="L9" s="4">
-        <v>0</v>
-      </c>
-      <c r="M9" s="4">
-        <v>0</v>
-      </c>
-      <c r="N9" s="4">
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4">
         <v>2</v>
       </c>
-      <c r="O9" s="4">
-        <v>0</v>
-      </c>
+      <c r="P15" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
OPERA Report - convert booking variables type
</commit_message>
<xml_diff>
--- a/Saudi/Booking.xlsx
+++ b/Saudi/Booking.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="26">
   <si>
     <t>Gender</t>
   </si>
@@ -72,7 +72,7 @@
     <t>Birth</t>
   </si>
   <si>
-    <t>VS</t>
+    <t>GC</t>
   </si>
   <si>
     <t>T</t>
@@ -81,19 +81,22 @@
     <t>CA</t>
   </si>
   <si>
+    <t>CHECKED IN</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
     <t>RESERVED</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>AE</t>
-  </si>
-  <si>
-    <t>RS</t>
-  </si>
-  <si>
-    <t>VI</t>
   </si>
 </sst>
 </file>
@@ -954,9 +957,7 @@
   </sheetPr>
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -967,16 +968,16 @@
     <col min="5" max="5" width="18.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="4.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="5.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="1" customWidth="1"/>
     <col min="10" max="10" width="7.85546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="11.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="10" style="1" customWidth="1"/>
     <col min="13" max="13" width="6.5703125" style="1" customWidth="1"/>
     <col min="14" max="14" width="13" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" style="1" customWidth="1"/>
     <col min="16" max="16" width="11" style="1" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5703125" style="1" customWidth="1"/>
     <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1057,7 +1058,9 @@
       <c r="I2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="3"/>
+      <c r="J2" s="4">
+        <v>1410</v>
+      </c>
       <c r="K2" s="5">
         <v>43548</v>
       </c>
@@ -1102,7 +1105,9 @@
       <c r="I3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="3"/>
+      <c r="J3" s="4">
+        <v>1410</v>
+      </c>
       <c r="K3" s="5">
         <v>43549</v>
       </c>
@@ -1147,7 +1152,9 @@
       <c r="I4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="3"/>
+      <c r="J4" s="4">
+        <v>1410</v>
+      </c>
       <c r="K4" s="5">
         <v>43550</v>
       </c>
@@ -1192,7 +1199,9 @@
       <c r="I5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="3"/>
+      <c r="J5" s="4">
+        <v>1410</v>
+      </c>
       <c r="K5" s="5">
         <v>43551</v>
       </c>
@@ -1237,7 +1246,9 @@
       <c r="I6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="3"/>
+      <c r="J6" s="4">
+        <v>1410</v>
+      </c>
       <c r="K6" s="5">
         <v>43552</v>
       </c>
@@ -1282,7 +1293,9 @@
       <c r="I7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="3"/>
+      <c r="J7" s="4">
+        <v>1410</v>
+      </c>
       <c r="K7" s="5">
         <v>43553</v>
       </c>
@@ -1329,7 +1342,7 @@
         <v>24</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J8" s="4">
         <v>401</v>
@@ -1380,7 +1393,7 @@
         <v>24</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J9" s="4">
         <v>401</v>
@@ -1431,7 +1444,7 @@
         <v>24</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J10" s="4">
         <v>401</v>
@@ -1482,7 +1495,7 @@
         <v>24</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J11" s="4">
         <v>401</v>
@@ -1533,7 +1546,7 @@
         <v>24</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J12" s="4">
         <v>401</v>
@@ -1584,7 +1597,7 @@
         <v>24</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J13" s="4">
         <v>401</v>
@@ -1635,7 +1648,7 @@
         <v>24</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J14" s="4">
         <v>401</v>
@@ -1686,7 +1699,7 @@
         <v>24</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J15" s="4">
         <v>401</v>

</xml_diff>

<commit_message>
OPERA Report - WIP in fetching cancel booking
</commit_message>
<xml_diff>
--- a/Saudi/Booking.xlsx
+++ b/Saudi/Booking.xlsx
@@ -19,7 +19,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
+  <si>
+    <t>Booking No</t>
+  </si>
+  <si>
+    <t>Birth</t>
+  </si>
   <si>
     <t>Gender</t>
   </si>
@@ -27,7 +33,13 @@
     <t>Nationality</t>
   </si>
   <si>
-    <t>Booking No</t>
+    <t>Ct</t>
+  </si>
+  <si>
+    <t>Pos</t>
+  </si>
+  <si>
+    <t>Pm</t>
   </si>
   <si>
     <t>Arrival Date</t>
@@ -36,42 +48,36 @@
     <t>Departure Date</t>
   </si>
   <si>
-    <t>Ct</t>
-  </si>
-  <si>
-    <t>Pos</t>
-  </si>
-  <si>
-    <t>Pm</t>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Res Date</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Disc</t>
+  </si>
+  <si>
+    <t>Disc Prcnt</t>
+  </si>
+  <si>
+    <t>Adults</t>
+  </si>
+  <si>
+    <t>Children</t>
   </si>
   <si>
     <t>Status</t>
   </si>
   <si>
-    <t>Room</t>
-  </si>
-  <si>
-    <t>Res Date</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>Disc</t>
-  </si>
-  <si>
-    <t>Disc Prcnt</t>
-  </si>
-  <si>
-    <t>Adults</t>
-  </si>
-  <si>
-    <t>Children</t>
-  </si>
-  <si>
-    <t>Birth</t>
-  </si>
-  <si>
     <t>GC</t>
   </si>
   <si>
@@ -81,16 +87,16 @@
     <t>CA</t>
   </si>
   <si>
+    <t>Deluxe King City View</t>
+  </si>
+  <si>
     <t>CHECKED IN</t>
   </si>
   <si>
+    <t>CT</t>
+  </si>
+  <si>
     <t>F</t>
-  </si>
-  <si>
-    <t>AE</t>
-  </si>
-  <si>
-    <t>RS</t>
   </si>
   <si>
     <t>VI</t>
@@ -240,21 +246,21 @@
     </font>
     <font>
       <b/>
-      <sz val="5"/>
+      <sz val="4"/>
       <color rgb="FF326598"/>
       <name val="Helvetica"/>
     </font>
     <font>
+      <sz val="4"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="5"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica"/>
     </font>
   </fonts>
   <fills count="36">
@@ -628,7 +634,7 @@
     <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="15" fontId="20" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="19" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -955,33 +961,37 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="13" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="11" style="1" customWidth="1"/>
-    <col min="17" max="17" width="8.5703125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="7.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="7.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1033,696 +1043,428 @@
       <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>24926</v>
       </c>
-      <c r="D2" s="5">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="5">
         <v>43548</v>
       </c>
-      <c r="E2" s="5">
+      <c r="I2" s="5">
         <v>43553</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="J2" s="3">
+        <v>1410</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="3">
+        <v>1</v>
+      </c>
+      <c r="M2" s="5">
+        <v>43548</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>1</v>
+      </c>
+      <c r="R2" s="3">
+        <v>0</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>24926</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="4">
+      <c r="G3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="5">
+        <v>43548</v>
+      </c>
+      <c r="I3" s="5">
+        <v>43553</v>
+      </c>
+      <c r="J3" s="3">
         <v>1410</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="3">
+        <v>1</v>
+      </c>
+      <c r="M3" s="5">
+        <v>43549</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>1</v>
+      </c>
+      <c r="R3" s="3">
+        <v>0</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>24926</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="5">
         <v>43548</v>
       </c>
-      <c r="L2" s="4">
-        <v>0</v>
-      </c>
-      <c r="M2" s="4">
-        <v>0</v>
-      </c>
-      <c r="N2" s="4">
-        <v>0</v>
-      </c>
-      <c r="O2" s="4">
+      <c r="I4" s="5">
+        <v>43553</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1410</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="3">
         <v>1</v>
       </c>
-      <c r="P2" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="3"/>
+      <c r="M4" s="5">
+        <v>43550</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>1</v>
+      </c>
+      <c r="R4" s="3">
+        <v>0</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>24926</v>
       </c>
-      <c r="D3" s="5">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="5">
         <v>43548</v>
       </c>
-      <c r="E3" s="5">
+      <c r="I5" s="5">
         <v>43553</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="J5" s="3">
+        <v>1410</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="3">
+        <v>1</v>
+      </c>
+      <c r="M5" s="5">
+        <v>43551</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>1</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>24926</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="4">
+      <c r="G6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="5">
+        <v>43548</v>
+      </c>
+      <c r="I6" s="5">
+        <v>43553</v>
+      </c>
+      <c r="J6" s="3">
         <v>1410</v>
       </c>
-      <c r="K3" s="5">
-        <v>43549</v>
-      </c>
-      <c r="L3" s="4">
-        <v>0</v>
-      </c>
-      <c r="M3" s="4">
-        <v>0</v>
-      </c>
-      <c r="N3" s="4">
-        <v>0</v>
-      </c>
-      <c r="O3" s="4">
+      <c r="K6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="3">
         <v>1</v>
       </c>
-      <c r="P3" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="3"/>
+      <c r="M6" s="5">
+        <v>43552</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>1</v>
+      </c>
+      <c r="R6" s="3">
+        <v>0</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>24926</v>
       </c>
-      <c r="D4" s="5">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="5">
         <v>43548</v>
       </c>
-      <c r="E4" s="5">
+      <c r="I7" s="5">
         <v>43553</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="J7" s="3">
         <v>1410</v>
       </c>
-      <c r="K4" s="5">
-        <v>43550</v>
-      </c>
-      <c r="L4" s="4">
-        <v>0</v>
-      </c>
-      <c r="M4" s="4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="4">
-        <v>0</v>
-      </c>
-      <c r="O4" s="4">
+      <c r="K7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="3">
         <v>1</v>
       </c>
-      <c r="P4" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="3"/>
+      <c r="M7" s="5">
+        <v>43553</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
+      <c r="P7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>1</v>
+      </c>
+      <c r="R7" s="3">
+        <v>0</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4">
-        <v>24926</v>
-      </c>
-      <c r="D5" s="5">
-        <v>43548</v>
-      </c>
-      <c r="E5" s="5">
-        <v>43553</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="4">
-        <v>1410</v>
-      </c>
-      <c r="K5" s="5">
-        <v>43551</v>
-      </c>
-      <c r="L5" s="4">
-        <v>0</v>
-      </c>
-      <c r="M5" s="4">
-        <v>0</v>
-      </c>
-      <c r="N5" s="4">
-        <v>0</v>
-      </c>
-      <c r="O5" s="4">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>10900</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="5">
+        <v>43773</v>
+      </c>
+      <c r="I8" s="5">
+        <v>43774</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="3">
+        <v>4</v>
+      </c>
+      <c r="M8" s="5">
+        <v>43773</v>
+      </c>
+      <c r="N8" s="3">
+        <v>2700.01</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3">
         <v>1</v>
       </c>
-      <c r="P5" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="3"/>
+      <c r="R8" s="3">
+        <v>0</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4">
-        <v>24926</v>
-      </c>
-      <c r="D6" s="5">
-        <v>43548</v>
-      </c>
-      <c r="E6" s="5">
-        <v>43553</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="4">
-        <v>1410</v>
-      </c>
-      <c r="K6" s="5">
-        <v>43552</v>
-      </c>
-      <c r="L6" s="4">
-        <v>0</v>
-      </c>
-      <c r="M6" s="4">
-        <v>0</v>
-      </c>
-      <c r="N6" s="4">
-        <v>0</v>
-      </c>
-      <c r="O6" s="4">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>10900</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="5">
+        <v>43773</v>
+      </c>
+      <c r="I9" s="5">
+        <v>43774</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="3">
+        <v>4</v>
+      </c>
+      <c r="M9" s="5">
+        <v>43774</v>
+      </c>
+      <c r="N9" s="3">
+        <v>2700.01</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0</v>
+      </c>
+      <c r="P9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3">
         <v>1</v>
       </c>
-      <c r="P6" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="3"/>
-    </row>
-    <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4">
-        <v>24926</v>
-      </c>
-      <c r="D7" s="5">
-        <v>43548</v>
-      </c>
-      <c r="E7" s="5">
-        <v>43553</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="4">
-        <v>1410</v>
-      </c>
-      <c r="K7" s="5">
-        <v>43553</v>
-      </c>
-      <c r="L7" s="4">
-        <v>0</v>
-      </c>
-      <c r="M7" s="4">
-        <v>0</v>
-      </c>
-      <c r="N7" s="4">
-        <v>0</v>
-      </c>
-      <c r="O7" s="4">
-        <v>1</v>
-      </c>
-      <c r="P7" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="3"/>
-    </row>
-    <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="4">
-        <v>24903</v>
-      </c>
-      <c r="D8" s="5">
-        <v>43737</v>
-      </c>
-      <c r="E8" s="5">
-        <v>43744</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="4">
-        <v>401</v>
-      </c>
-      <c r="K8" s="5">
-        <v>43737</v>
-      </c>
-      <c r="L8" s="4">
-        <v>636.98</v>
-      </c>
-      <c r="M8" s="4">
-        <v>0</v>
-      </c>
-      <c r="N8" s="4">
-        <v>0</v>
-      </c>
-      <c r="O8" s="4">
-        <v>2</v>
-      </c>
-      <c r="P8" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="3"/>
-    </row>
-    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="4">
-        <v>24903</v>
-      </c>
-      <c r="D9" s="5">
-        <v>43737</v>
-      </c>
-      <c r="E9" s="5">
-        <v>43744</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="4">
-        <v>401</v>
-      </c>
-      <c r="K9" s="5">
-        <v>43738</v>
-      </c>
-      <c r="L9" s="4">
-        <v>636.98</v>
-      </c>
-      <c r="M9" s="4">
-        <v>0</v>
-      </c>
-      <c r="N9" s="4">
-        <v>0</v>
-      </c>
-      <c r="O9" s="4">
-        <v>2</v>
-      </c>
-      <c r="P9" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="3"/>
-    </row>
-    <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="4">
-        <v>24903</v>
-      </c>
-      <c r="D10" s="5">
-        <v>43737</v>
-      </c>
-      <c r="E10" s="5">
-        <v>43744</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="4">
-        <v>401</v>
-      </c>
-      <c r="K10" s="5">
-        <v>43739</v>
-      </c>
-      <c r="L10" s="4">
-        <v>696.83</v>
-      </c>
-      <c r="M10" s="4">
-        <v>0</v>
-      </c>
-      <c r="N10" s="4">
-        <v>0</v>
-      </c>
-      <c r="O10" s="4">
-        <v>2</v>
-      </c>
-      <c r="P10" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="3"/>
-    </row>
-    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="4">
-        <v>24903</v>
-      </c>
-      <c r="D11" s="5">
-        <v>43737</v>
-      </c>
-      <c r="E11" s="5">
-        <v>43744</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" s="4">
-        <v>401</v>
-      </c>
-      <c r="K11" s="5">
-        <v>43740</v>
-      </c>
-      <c r="L11" s="4">
-        <v>696.83</v>
-      </c>
-      <c r="M11" s="4">
-        <v>0</v>
-      </c>
-      <c r="N11" s="4">
-        <v>0</v>
-      </c>
-      <c r="O11" s="4">
-        <v>2</v>
-      </c>
-      <c r="P11" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="3"/>
-    </row>
-    <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="4">
-        <v>24903</v>
-      </c>
-      <c r="D12" s="5">
-        <v>43737</v>
-      </c>
-      <c r="E12" s="5">
-        <v>43744</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="4">
-        <v>401</v>
-      </c>
-      <c r="K12" s="5">
-        <v>43741</v>
-      </c>
-      <c r="L12" s="4">
-        <v>696.83</v>
-      </c>
-      <c r="M12" s="4">
-        <v>0</v>
-      </c>
-      <c r="N12" s="4">
-        <v>0</v>
-      </c>
-      <c r="O12" s="4">
-        <v>2</v>
-      </c>
-      <c r="P12" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="3"/>
-    </row>
-    <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="4">
-        <v>24903</v>
-      </c>
-      <c r="D13" s="5">
-        <v>43737</v>
-      </c>
-      <c r="E13" s="5">
-        <v>43744</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J13" s="4">
-        <v>401</v>
-      </c>
-      <c r="K13" s="5">
-        <v>43742</v>
-      </c>
-      <c r="L13" s="4">
-        <v>696.83</v>
-      </c>
-      <c r="M13" s="4">
-        <v>0</v>
-      </c>
-      <c r="N13" s="4">
-        <v>0</v>
-      </c>
-      <c r="O13" s="4">
-        <v>2</v>
-      </c>
-      <c r="P13" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="3"/>
-    </row>
-    <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="4">
-        <v>24903</v>
-      </c>
-      <c r="D14" s="5">
-        <v>43737</v>
-      </c>
-      <c r="E14" s="5">
-        <v>43744</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J14" s="4">
-        <v>401</v>
-      </c>
-      <c r="K14" s="5">
-        <v>43743</v>
-      </c>
-      <c r="L14" s="4">
-        <v>696.83</v>
-      </c>
-      <c r="M14" s="4">
-        <v>0</v>
-      </c>
-      <c r="N14" s="4">
-        <v>0</v>
-      </c>
-      <c r="O14" s="4">
-        <v>2</v>
-      </c>
-      <c r="P14" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="3"/>
-    </row>
-    <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="4">
-        <v>24903</v>
-      </c>
-      <c r="D15" s="5">
-        <v>43737</v>
-      </c>
-      <c r="E15" s="5">
-        <v>43744</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15" s="4">
-        <v>401</v>
-      </c>
-      <c r="K15" s="5">
-        <v>43744</v>
-      </c>
-      <c r="L15" s="4">
-        <v>696.83</v>
-      </c>
-      <c r="M15" s="4">
-        <v>0</v>
-      </c>
-      <c r="N15" s="4">
-        <v>0</v>
-      </c>
-      <c r="O15" s="4">
-        <v>2</v>
-      </c>
-      <c r="P15" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="3"/>
+      <c r="R9" s="3">
+        <v>0</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>